<commit_message>
Updated R markdown, removed irrelevant files
</commit_message>
<xml_diff>
--- a/Avariegatum_seq/03_cameroonticks/14_Ra_snp/251017_pca/meta.xlsx
+++ b/Avariegatum_seq/03_cameroonticks/14_Ra_snp/251017_pca/meta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jing/Library/CloudStorage/OneDrive-Personal/Avariegatum_seq/03_cameroonticks/14_Ra_snp/251017_pca/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a575da6b6b23e7/AVL/Avariegatum_seq/03_cameroonticks/14_Ra_snp/251017_pca/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F626B8A7-6240-FC45-BEF0-905FD7D455B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{F626B8A7-6240-FC45-BEF0-905FD7D455B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19690061-60F9-1447-8C42-6E4EF0AB6F0F}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="760" windowWidth="28860" windowHeight="18880" xr2:uid="{CCD7B65F-D414-034F-AB16-CD91D6E4CC89}"/>
+    <workbookView xWindow="1500" yWindow="760" windowWidth="28740" windowHeight="18880" xr2:uid="{CCD7B65F-D414-034F-AB16-CD91D6E4CC89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -572,7 +572,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>